<commit_message>
- Aggiunti filtri anche su Abilita e filtri multipli. - predisposto per deploy su onrender
</commit_message>
<xml_diff>
--- a/ffta_backend/data/job.xlsx
+++ b/ffta_backend/data/job.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sviluppo\FFTA_Tracking\ffta_backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30348F37-6AC6-4D85-B117-380CBCFC9FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF39056-D475-45EF-912E-1055C94621CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="555" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -696,6 +696,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="109.42578125" style="3" customWidth="1"/>
   </cols>
@@ -1025,7 +1026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>129</v>
       </c>
@@ -1057,7 +1058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>130</v>
       </c>
@@ -1086,7 +1087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>131</v>
       </c>
@@ -1118,7 +1119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>132</v>
       </c>
@@ -1147,7 +1148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>133</v>
       </c>
@@ -1182,7 +1183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>134</v>
       </c>
@@ -1217,7 +1218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>135</v>
       </c>
@@ -1249,7 +1250,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>136</v>
       </c>
@@ -1278,7 +1279,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>151</v>
       </c>
@@ -1307,7 +1308,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>152</v>
       </c>
@@ -1336,7 +1337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>153</v>
       </c>
@@ -1365,7 +1366,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>155</v>
       </c>
@@ -1394,7 +1395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>156</v>
       </c>
@@ -1423,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="240" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>158</v>
       </c>
@@ -1455,7 +1456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>172</v>
       </c>
@@ -1484,7 +1485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>173</v>
       </c>
@@ -1513,7 +1514,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>177</v>
       </c>
@@ -1542,7 +1543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>179</v>
       </c>
@@ -1571,7 +1572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>195</v>
       </c>
@@ -1600,7 +1601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>196</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>198</v>
       </c>
@@ -1658,7 +1659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>200</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>201</v>
       </c>
@@ -1716,7 +1717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>202</v>
       </c>

</xml_diff>